<commit_message>
Update: fixed bounds not updating properly in S.bo
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{854F8A39-8242-4658-8F6B-FB84C28082C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CD28D5FC-35EF-4B34-A034-2974969685B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -636,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B78F5ED-0798-4D77-8F9F-1DE91C850719}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -670,7 +670,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -693,7 +693,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -716,7 +716,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -739,7 +739,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -762,7 +762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -785,15 +785,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>8.9922067541464052</v>
+        <v>0.89922067541464101</v>
       </c>
       <c r="B7">
-        <v>7.99307267035236</v>
+        <v>0.1</v>
       </c>
       <c r="C7">
-        <v>7.99307267035236</v>
+        <v>0.1</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -808,7 +808,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -831,7 +831,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2.5</v>
       </c>
@@ -854,18 +854,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.21999999999999997</v>
       </c>
       <c r="B10">
-        <v>0.12635382862630201</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.12635382862630201</v>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="C10">
+        <v>0.21999999999999997</v>
       </c>
       <c r="D10">
-        <v>0.12635382862630201</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="E10" s="1">
         <v>0.22</v>
@@ -876,8 +876,17 @@
       <c r="G10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>0.12635382862630201</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.12635382862630201</v>
+      </c>
+      <c r="K10">
+        <v>0.12635382862630201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.623</v>
       </c>
@@ -900,7 +909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -923,7 +932,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
@@ -946,11 +955,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0</v>
       </c>
       <c r="C14">
@@ -969,7 +978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.2</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.3</v>
       </c>
@@ -1066,10 +1075,10 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1089,10 +1098,10 @@
         <v>0.156</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.156</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.156</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1391,7 +1400,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,10 +1827,10 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1841,10 +1850,10 @@
         <v>2.2699999999999999E-3</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2142,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -2173,6 +2182,7 @@
       <c r="C2" t="s">
         <v>61</v>
       </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -2184,6 +2194,7 @@
       <c r="C3" t="s">
         <v>62</v>
       </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -2195,10 +2206,11 @@
       <c r="C4" t="s">
         <v>63</v>
       </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -2206,10 +2218,11 @@
       <c r="C5" t="s">
         <v>64</v>
       </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2217,10 +2230,13 @@
       <c r="C6" t="s">
         <v>67</v>
       </c>
+      <c r="F6" s="2">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>100</v>
@@ -2229,15 +2245,14 @@
         <v>65</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>150</v>
       </c>
       <c r="B8" s="2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C8" t="s">
         <v>66</v>
@@ -2248,7 +2263,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
@@ -2256,22 +2271,21 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>4.32</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>21.065000000000001</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2360,8 +2374,7 @@
         <v>0.47199999999999998</v>
       </c>
       <c r="B19" s="2">
-        <f>D19*10</f>
-        <v>0</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
@@ -2479,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="2">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
@@ -2525,7 +2538,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,7 +2594,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Dynamic block now runs as loop instead of hard coding each metabolite/statevar
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CD28D5FC-35EF-4B34-A034-2974969685B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02FB2C8D-8BDD-46E4-81C3-E434CC094D04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
@@ -2151,9 +2151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2161,9 +2159,9 @@
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2">
         <v>5</v>
@@ -2172,59 +2170,79 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>10.9</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="F2" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="F3" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="F4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
@@ -2233,162 +2251,207 @@
       <c r="F6" s="2">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>100</v>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>150</v>
       </c>
-      <c r="B8" s="2">
-        <v>500</v>
+      <c r="B8">
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>50</v>
+      <c r="B9">
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
-        <v>200</v>
+      <c r="B10">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>20</v>
       </c>
-      <c r="B11" s="2">
-        <v>100</v>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
-        <v>2</v>
+      <c r="B12">
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>4.4710000000000001</v>
       </c>
-      <c r="B13" s="2">
-        <v>4.4710000000000001</v>
+      <c r="B13">
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2">
+        <v>4.4710000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1.4079999999999999</v>
       </c>
-      <c r="B14" s="2">
-        <v>1.4079999999999999</v>
+      <c r="B14">
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <v>1.4079999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3.4910000000000001</v>
       </c>
-      <c r="B15" s="2">
-        <v>3.4910000000000001</v>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="2">
+        <v>3.4910000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2.2120000000000002</v>
       </c>
-      <c r="B16" s="2">
-        <v>2.2120000000000002</v>
+      <c r="B16">
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.2120000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>3.4609999999999999</v>
       </c>
-      <c r="B17" s="2">
-        <v>3.4609999999999999</v>
+      <c r="B17">
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3.4609999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2.7629999999999999</v>
       </c>
-      <c r="B18" s="2">
-        <v>2.7629999999999999</v>
+      <c r="B18">
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2.7629999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>0.47199999999999998</v>
       </c>
-      <c r="B19" s="2">
-        <v>0.47199999999999998</v>
+      <c r="B19">
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.47199999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1.2589999999999999</v>
       </c>
-      <c r="B20" s="2">
-        <v>1.2589999999999999</v>
+      <c r="B20">
+        <v>0</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.2589999999999999</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
@@ -2398,11 +2461,14 @@
       <c r="A21" s="2">
         <v>5.0979999999999999</v>
       </c>
-      <c r="B21" s="2">
-        <v>5.0979999999999999</v>
+      <c r="B21">
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
+      </c>
+      <c r="G21" s="2">
+        <v>5.0979999999999999</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
@@ -2411,11 +2477,14 @@
       <c r="A22" s="2">
         <v>2.734</v>
       </c>
-      <c r="B22" s="2">
-        <v>2.734</v>
+      <c r="B22">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2.734</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
@@ -2424,100 +2493,127 @@
       <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
       </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>0</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
       </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>0</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>0</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
       </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
         <v>54</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
         <v>55</v>
       </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>0</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
       </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>0</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>57</v>
       </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>0</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix:deleted a few extra lines in last commit
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02FB2C8D-8BDD-46E4-81C3-E434CC094D04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9CCC8F8E-9CA8-46A8-BDBE-46EF3237E2F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
@@ -2151,7 +2151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2172,7 +2174,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="B2">
         <v>0</v>

</xml_diff>

<commit_message>
Update: new function checkFluxes & other
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9CCC8F8E-9CA8-46A8-BDBE-46EF3237E2F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{961DF506-CA4C-418A-9150-D971E26BD77C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="83">
   <si>
     <t>sbo</t>
   </si>
@@ -48,192 +48,6 @@
     <t>col</t>
   </si>
   <si>
-    <t>x(7):Glucose (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(8):Water (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(9):Oxygen (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(10):Phosphate (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(11):Ammonium (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(12):Acetate (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(13):Glutamine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(14):Histidine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(15):Lysine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(16):Phenylalanine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(17):Valine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(18):Threonine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(19):Tryptophan (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(20):Methionine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(21):Leucine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(22):Isoleucine (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(23):Carbon dioxide (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(24):Propanoate (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(25):Butyrate (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(28):Methane (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(29):MFalpha2 (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(30):Myrosinase (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(31):P28 (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(26):Succinate (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(27):Ethanol (mmol/L)</t>
-  </si>
-  <si>
-    <t>x(1):S.bo biomass (g/L)</t>
-  </si>
-  <si>
-    <t>x(2):B.th biomass (g/L)</t>
-  </si>
-  <si>
-    <t>x(3):E.re biomass (g/L)</t>
-  </si>
-  <si>
-    <t>x(4):M.si biomass (g/L)</t>
-  </si>
-  <si>
-    <t>x(5):Cancer biomass (g/L)</t>
-  </si>
-  <si>
-    <t>x(6):Colon biomass (g/L)</t>
-  </si>
-  <si>
-    <t>x(10):Phosphate</t>
-  </si>
-  <si>
-    <t>x(11):Ammonium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(12):Acetate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(13):Glutamine </t>
-  </si>
-  <si>
-    <t>x(14):Histidine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(15):Lysine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(16):Phenylalanine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(17):Valine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(18):Threonine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(19):Tryptophan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(20):Methionine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(21):Leucine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(22):Isoleucine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(23):Carbon dioxide </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(24):Propanoate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(25):Butyrate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(26):Succinate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(27):Ethanol </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(28):Methane </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(29):MFalpha2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(30):Myrosinase </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(31):P28 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(9):Oxygen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(1):S.bo biomass </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(2):B.th biomass </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(3):E.re biomass </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(4):M.si biomass </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(5):Cancer biomass </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(7):Glucose </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(8):Water </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(6):Colon biomass </t>
-  </si>
-  <si>
     <t>Initial Condition</t>
   </si>
   <si>
@@ -271,6 +85,198 @@
   </si>
   <si>
     <t>Dilution rate (F/V)</t>
+  </si>
+  <si>
+    <t>x(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.bo biomass </t>
+  </si>
+  <si>
+    <t>x(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.th biomass </t>
+  </si>
+  <si>
+    <t>x(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.re biomass </t>
+  </si>
+  <si>
+    <t>x(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.si biomass </t>
+  </si>
+  <si>
+    <t>x(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancer biomass </t>
+  </si>
+  <si>
+    <t>x(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colon biomass </t>
+  </si>
+  <si>
+    <t>x(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glucose </t>
+  </si>
+  <si>
+    <t>x(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water </t>
+  </si>
+  <si>
+    <t>x(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen </t>
+  </si>
+  <si>
+    <t>x(10)</t>
+  </si>
+  <si>
+    <t>Phosphate</t>
+  </si>
+  <si>
+    <t>x(11)</t>
+  </si>
+  <si>
+    <t>Ammonium</t>
+  </si>
+  <si>
+    <t>x(13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutamine </t>
+  </si>
+  <si>
+    <t>x(14)</t>
+  </si>
+  <si>
+    <t>Histidine</t>
+  </si>
+  <si>
+    <t>x(15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lysine </t>
+  </si>
+  <si>
+    <t>x(16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenylalanine </t>
+  </si>
+  <si>
+    <t>x(17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valine </t>
+  </si>
+  <si>
+    <t>x(18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threonine </t>
+  </si>
+  <si>
+    <t>x(19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tryptophan </t>
+  </si>
+  <si>
+    <t>x(20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methionine </t>
+  </si>
+  <si>
+    <t>x(21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leucine </t>
+  </si>
+  <si>
+    <t>x(22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isoleucine </t>
+  </si>
+  <si>
+    <t>x(23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetate </t>
+  </si>
+  <si>
+    <t>x(24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon dioxide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propanoate </t>
+  </si>
+  <si>
+    <t>x(25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butyrate </t>
+  </si>
+  <si>
+    <t>x(26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Succinate </t>
+  </si>
+  <si>
+    <t>x(27)</t>
+  </si>
+  <si>
+    <t>Formate</t>
+  </si>
+  <si>
+    <t>x(28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethanol </t>
+  </si>
+  <si>
+    <t>x(29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane </t>
+  </si>
+  <si>
+    <t>x(30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFalpha2 </t>
+  </si>
+  <si>
+    <t>x(31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myrosinase </t>
+  </si>
+  <si>
+    <t>x(32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P28 </t>
+  </si>
+  <si>
+    <t>x(12)</t>
   </si>
 </sst>
 </file>
@@ -636,18 +642,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B78F5ED-0798-4D77-8F9F-1DE91C850719}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -667,10 +673,13 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -690,10 +699,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -713,10 +725,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -736,10 +751,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -759,10 +777,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -782,18 +803,21 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.89922067541464101</v>
-      </c>
-      <c r="B7">
-        <v>0.1</v>
-      </c>
-      <c r="C7">
-        <v>0.1</v>
+        <v>8.9922067541464106</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.9922067541464106</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.9922067541464106</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -805,10 +829,13 @@
         <v>1.04895</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -828,10 +855,13 @@
         <v>1000</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2.5</v>
       </c>
@@ -851,42 +881,48 @@
         <v>8.7585034013605458</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.21999999999999997</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="B10">
-        <v>0.21999999999999997</v>
+        <v>0.126</v>
       </c>
       <c r="C10">
-        <v>0.21999999999999997</v>
+        <v>0.126</v>
       </c>
       <c r="D10">
-        <v>0.21999999999999997</v>
+        <v>0.126</v>
       </c>
       <c r="E10" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="I10">
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10">
         <v>0.12635382862630201</v>
       </c>
-      <c r="J10" s="1">
+      <c r="M10" s="1">
         <v>0.12635382862630201</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>0.12635382862630201</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.623</v>
       </c>
@@ -906,12 +942,15 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -919,24 +958,27 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" s="1">
-        <v>6.6087133343500586</v>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>2.0625000000000001E-2</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13">
@@ -952,14 +994,17 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
@@ -975,12 +1020,15 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.2</v>
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.3</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -998,12 +1046,15 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.3</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1021,12 +1072,15 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0.56399999999999995</v>
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.2</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1044,18 +1098,21 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.2</v>
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.23599999999999999</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1067,18 +1124,21 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.23599999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="B19">
-        <v>0.23599999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="C19">
-        <v>0.23599999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1090,18 +1150,21 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.156</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="B20">
-        <v>0.156</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0.156</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1113,12 +1176,15 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.63200000000000001</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1136,12 +1202,15 @@
         <v>2.0625000000000001E-2</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.38400000000000001</v>
+        <v>0</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1150,42 +1219,48 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E22">
-        <v>0.20625000000000002</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>2.0625000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
+        <v>59</v>
+      </c>
+      <c r="H22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>0</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>2.5</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
+        <v>6.6</v>
+      </c>
+      <c r="D23" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.7160000000000002E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.7160000000000002E-2</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1199,16 +1274,19 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>6.5399999999999998E-3</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>6.5399999999999998E-3</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1218,20 +1296,23 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.1220000000000001E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.1220000000000001E-2</v>
       </c>
       <c r="G25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1239,22 +1320,25 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>6.6</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1264,20 +1348,23 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
+      <c r="D27" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1297,10 +1384,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1320,10 +1410,13 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1343,10 +1436,13 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1366,26 +1462,55 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>3</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1397,18 +1522,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A256C0EB-A98E-4A67-AA7F-D6B1D6307FBC}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="G1" sqref="G1:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1428,10 +1553,13 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1451,10 +1579,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1474,10 +1605,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1497,10 +1631,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1520,10 +1657,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1543,33 +1683,39 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.31084171495814739</v>
       </c>
-      <c r="B7">
-        <v>2.7753724549834589E-4</v>
-      </c>
-      <c r="C7">
-        <v>2.7753724549834589E-4</v>
+      <c r="B7" s="1">
+        <v>0.31084171495814739</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.31084171495814739</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1.5</v>
+        <v>1.05</v>
       </c>
       <c r="F7" s="1">
-        <v>1.5</v>
+        <v>1.05</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1E-3</v>
       </c>
@@ -1589,10 +1735,13 @@
         <v>1E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1612,10 +1761,13 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.157</v>
       </c>
@@ -1635,10 +1787,13 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1658,12 +1813,15 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.2199999999999999E-3</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1672,19 +1830,22 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.33890837612051583</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -1694,20 +1855,23 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>0.24</v>
       </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="F13" s="1">
+        <v>0.24</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -1727,12 +1891,15 @@
         <v>0.24</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1.2199999999999999E-3</v>
+        <v>7.2000000000000005E-4</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1750,12 +1917,15 @@
         <v>0.24</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>7.2000000000000005E-4</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1773,12 +1943,15 @@
         <v>0.24</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>8.0000000000000002E-3</v>
+        <v>1.2199999999999999E-3</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1796,18 +1969,21 @@
         <v>0.24</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1.2199999999999999E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1819,18 +1995,21 @@
         <v>0.24</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>8.9999999999999998E-4</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="B19">
-        <v>8.9999999999999998E-4</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="C19">
-        <v>8.9999999999999998E-4</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1842,18 +2021,21 @@
         <v>0.24</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2.2699999999999999E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="B20">
-        <v>2.2699999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>2.2699999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1865,12 +2047,15 @@
         <v>0.24</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1.07E-3</v>
+        <v>1.2199999999999999E-3</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1888,12 +2073,15 @@
         <v>0.24</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1.2199999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1901,43 +2089,49 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22">
-        <v>0</v>
+      <c r="D22" s="2">
+        <v>0.02</v>
       </c>
       <c r="E22" s="1">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
+      <c r="C23" s="1">
+        <v>0.33890837612051583</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.33890837612051583</v>
+      </c>
+      <c r="E23">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="F23">
+        <v>0.56499999999999995</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1951,16 +2145,19 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1977,21 +2174,24 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" s="1">
+        <v>0.33890837612051583</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2003,11 +2203,14 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
+        <v>68</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>0</v>
       </c>
       <c r="B27">
@@ -2016,20 +2219,23 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
+      <c r="D27" s="1">
+        <v>0.33890837612051583</v>
+      </c>
+      <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2049,10 +2255,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2072,10 +2281,13 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2095,10 +2307,13 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2118,26 +2333,55 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>3</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2149,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,297 +2407,287 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>5.5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
+      <c r="A3" s="2">
+        <v>10.9</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="2">
-        <v>10.9</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
+      <c r="A4" s="2">
+        <v>0.3</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
+      <c r="A5" s="2">
+        <v>1E-3</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" s="2">
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>100</v>
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>150</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="B8" s="2">
+        <v>500</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="2">
-        <v>500</v>
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" s="2">
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="2">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" s="2">
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="2">
-        <v>200</v>
+      <c r="D10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="B11" s="2">
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="2">
-        <v>100</v>
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.4710000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="G12" s="2">
-        <v>2</v>
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>4.4710000000000001</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.4079999999999999</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="2">
-        <v>4.4710000000000001</v>
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>1.4079999999999999</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
+        <v>3.4910000000000001</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.4910000000000001</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1.4079999999999999</v>
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>3.4910000000000001</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
+        <v>2.2120000000000002</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2.2120000000000002</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="2">
-        <v>3.4910000000000001</v>
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>2.2120000000000002</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
+        <v>3.4609999999999999</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3.4609999999999999</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="2">
-        <v>2.2120000000000002</v>
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>3.4609999999999999</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.7629999999999999</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="2">
-        <v>3.4609999999999999</v>
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>2.7629999999999999</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.47199999999999998</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="2">
-        <v>2.7629999999999999</v>
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.2589999999999999</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.47199999999999998</v>
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>1.2589999999999999</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
+        <v>5.0979999999999999</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5.0979999999999999</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1.2589999999999999</v>
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
@@ -2461,48 +2695,48 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>5.0979999999999999</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
+        <v>2.734</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.734</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="2">
-        <v>5.0979999999999999</v>
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>2.734</v>
-      </c>
-      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="2">
-        <v>2.734</v>
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
       </c>
       <c r="K23" s="3"/>
     </row>
@@ -2510,120 +2744,134 @@
       <c r="A24" s="2">
         <v>0</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>0</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>0</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>1</v>
-      </c>
-      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>0</v>
-      </c>
-      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>0</v>
       </c>
-      <c r="B30">
-        <v>0</v>
+      <c r="B30" s="2">
+        <v>1E-3</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>0</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" t="s">
-        <v>69</v>
+      <c r="A32" s="2">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2650,13 +2898,13 @@
         <v>7.7999999999999996E-3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -2665,13 +2913,13 @@
         <v>1000</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -2680,13 +2928,13 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -2695,13 +2943,13 @@
         <v>0.01</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updating paramTables.xlsx (currently set to only Sbo in batch)
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{961DF506-CA4C-418A-9150-D971E26BD77C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CCD1509-A3E9-4523-93ED-BDEA94D8180F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B78F5ED-0798-4D77-8F9F-1DE91C850719}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G11" t="s">
         <v>39</v>
@@ -1525,7 +1525,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H32"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="B11" s="1">
         <v>3.0000000000000001E-3</v>
@@ -1810,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G11" t="s">
         <v>39</v>
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="F25">
         <v>8.2000000000000003E-2</v>
@@ -2395,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,12 +2405,12 @@
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -2418,10 +2418,16 @@
       <c r="D1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>5.5</v>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2432,11 +2438,16 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>10.9</v>
+      <c r="G2" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2447,11 +2458,16 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>0.3</v>
+      <c r="G3" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2462,11 +2478,16 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1E-3</v>
+      <c r="G4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2477,11 +2498,16 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1.7</v>
+      <c r="G5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2492,14 +2518,19 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>100</v>
+      <c r="G6" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2507,13 +2538,19 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="G7" s="2">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2">
         <v>100</v>
       </c>
-      <c r="B8" s="2">
-        <v>500</v>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2521,13 +2558,19 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
-        <v>50</v>
+      <c r="G8" s="2">
+        <v>100</v>
+      </c>
+      <c r="H8" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -2535,13 +2578,19 @@
       <c r="D9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="G9" s="2">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
-        <v>200</v>
+      <c r="H9" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -2549,13 +2598,19 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2">
-        <v>100</v>
+      <c r="G10" s="2">
+        <v>10</v>
+      </c>
+      <c r="H10" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
@@ -2563,13 +2618,19 @@
       <c r="D11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>4.4710000000000001</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4.4710000000000001</v>
+      <c r="G11" s="2">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -2577,13 +2638,19 @@
       <c r="D12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1.4079999999999999</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1.4079999999999999</v>
+      <c r="G12" s="2">
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.4710000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -2591,13 +2658,19 @@
       <c r="D13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>3.4910000000000001</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3.4910000000000001</v>
+      <c r="G13" s="2">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.4079999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
@@ -2605,13 +2678,19 @@
       <c r="D14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2.2120000000000002</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2.2120000000000002</v>
+      <c r="G14" s="2">
+        <v>3.4910000000000001</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3.4910000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>45</v>
@@ -2619,13 +2698,19 @@
       <c r="D15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>3.4609999999999999</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3.4609999999999999</v>
+      <c r="G15" s="2">
+        <v>2.2120000000000002</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2.2120000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -2633,13 +2718,19 @@
       <c r="D16" t="s">
         <v>50</v>
       </c>
+      <c r="G16" s="2">
+        <v>3.4609999999999999</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3.4609999999999999</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2.7629999999999999</v>
-      </c>
-      <c r="B17" s="2">
-        <v>2.7629999999999999</v>
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>49</v>
@@ -2647,13 +2738,19 @@
       <c r="D17" t="s">
         <v>52</v>
       </c>
+      <c r="G17" s="2">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2.7629999999999999</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.47199999999999998</v>
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -2661,13 +2758,19 @@
       <c r="D18" t="s">
         <v>54</v>
       </c>
+      <c r="G18" s="2">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.47199999999999998</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1.2589999999999999</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1.2589999999999999</v>
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>53</v>
@@ -2675,30 +2778,42 @@
       <c r="D19" t="s">
         <v>56</v>
       </c>
+      <c r="G19" s="2">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.2589999999999999</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>5.0979999999999999</v>
-      </c>
-      <c r="B20" s="2">
-        <v>5.0979999999999999</v>
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
       </c>
       <c r="D20" t="s">
         <v>58</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5.0979999999999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.0979999999999999</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2.734</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2.734</v>
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -2706,14 +2821,20 @@
       <c r="D21" t="s">
         <v>60</v>
       </c>
+      <c r="G21" s="2">
+        <v>2.734</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2.734</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" t="s">
@@ -2722,14 +2843,20 @@
       <c r="D22" t="s">
         <v>64</v>
       </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>0</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" t="s">
@@ -2738,13 +2865,19 @@
       <c r="D23" t="s">
         <v>62</v>
       </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
@@ -2753,12 +2886,18 @@
       <c r="D24" t="s">
         <v>65</v>
       </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>0</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
@@ -2767,12 +2906,18 @@
       <c r="D25" t="s">
         <v>67</v>
       </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>0</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" t="s">
@@ -2781,12 +2926,18 @@
       <c r="D26" t="s">
         <v>69</v>
       </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>0</v>
-      </c>
-      <c r="B27" s="2">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
@@ -2795,12 +2946,18 @@
       <c r="D27" t="s">
         <v>71</v>
       </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>0</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
@@ -2809,12 +2966,18 @@
       <c r="D28" t="s">
         <v>73</v>
       </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
@@ -2823,13 +2986,19 @@
       <c r="D29" t="s">
         <v>75</v>
       </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>0</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1E-3</v>
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>76</v>
@@ -2837,12 +3006,18 @@
       <c r="D30" t="s">
         <v>77</v>
       </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" t="s">
@@ -2851,12 +3026,18 @@
       <c r="D31" t="s">
         <v>79</v>
       </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" t="s">
@@ -2864,6 +3045,12 @@
       </c>
       <c r="D32" t="s">
         <v>81</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update: Added new function updateFluxes() and finxed critical bound-updating problem in function f()
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CCD1509-A3E9-4523-93ED-BDEA94D8180F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7BF8F8E5-AAD6-45E4-B25B-142C4BAAF2A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -642,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B78F5ED-0798-4D77-8F9F-1DE91C850719}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q14:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,7 @@
     <col min="7" max="7" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -757,7 +757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -783,7 +783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -809,7 +809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>8.9922067541464106</v>
       </c>
@@ -835,7 +835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -846,7 +846,7 @@
         <v>1000</v>
       </c>
       <c r="D8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1000</v>
@@ -861,7 +861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2.5</v>
       </c>
@@ -887,7 +887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -895,10 +895,10 @@
         <v>0.126</v>
       </c>
       <c r="C10">
-        <v>0.126</v>
+        <v>1.26</v>
       </c>
       <c r="D10">
-        <v>0.126</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1">
         <v>2.1999999999999999E-2</v>
@@ -912,17 +912,9 @@
       <c r="H10" t="s">
         <v>38</v>
       </c>
-      <c r="L10">
-        <v>0.12635382862630201</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0.12635382862630201</v>
-      </c>
-      <c r="N10">
-        <v>0.12635382862630201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.623</v>
       </c>
@@ -948,24 +940,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.2</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E12">
         <v>0.20625000000000002</v>
       </c>
       <c r="F12">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G12" t="s">
         <v>82</v>
@@ -974,24 +966,24 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
+      <c r="B13">
+        <v>0.20625000000000002</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E13">
         <v>0.20625000000000002</v>
       </c>
       <c r="F13">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G13" t="s">
         <v>41</v>
@@ -1000,24 +992,24 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E14">
         <v>0.20625000000000002</v>
       </c>
       <c r="F14">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G14" t="s">
         <v>43</v>
@@ -1026,24 +1018,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.3</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E15">
         <v>0.20625000000000002</v>
       </c>
       <c r="F15">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G15" t="s">
         <v>45</v>
@@ -1052,24 +1044,24 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.56399999999999995</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E16">
         <v>0.20625000000000002</v>
       </c>
       <c r="F16">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G16" t="s">
         <v>47</v>
@@ -1083,19 +1075,19 @@
         <v>0.2</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E17">
         <v>0.20625000000000002</v>
       </c>
       <c r="F17">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G17" t="s">
         <v>49</v>
@@ -1115,13 +1107,13 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E18">
         <v>0.20625000000000002</v>
       </c>
       <c r="F18">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G18" t="s">
         <v>51</v>
@@ -1141,13 +1133,13 @@
         <v>0.156</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E19">
         <v>0.20625000000000002</v>
       </c>
       <c r="F19">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G19" t="s">
         <v>53</v>
@@ -1161,19 +1153,19 @@
         <v>0.63200000000000001</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E20">
         <v>0.20625000000000002</v>
       </c>
       <c r="F20">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G20" t="s">
         <v>55</v>
@@ -1187,19 +1179,19 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="E21">
         <v>0.20625000000000002</v>
       </c>
       <c r="F21">
-        <v>2.0625000000000001E-2</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="G21" t="s">
         <v>57</v>
@@ -1369,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1525,7 +1517,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,7 +1718,7 @@
         <v>1E-3</v>
       </c>
       <c r="D8">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1E-3</v>
@@ -1823,20 +1815,20 @@
       <c r="A12">
         <v>1.2199999999999999E-3</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="B12" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.24</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="E12" s="1">
         <v>0.24</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" s="1">
+        <v>0.24</v>
       </c>
       <c r="G12" t="s">
         <v>82</v>
@@ -1849,14 +1841,14 @@
       <c r="A13">
         <v>1.2199999999999999E-3</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+      <c r="B13" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="E13" s="1">
         <v>0.24</v>
@@ -1875,14 +1867,14 @@
       <c r="A14">
         <v>1.2199999999999999E-3</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="B14" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="E14" s="1">
         <v>0.24</v>
@@ -1901,14 +1893,14 @@
       <c r="A15">
         <v>7.2000000000000005E-4</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="B15" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="E15" s="1">
         <v>0.24</v>
@@ -1927,14 +1919,14 @@
       <c r="A16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+      <c r="B16" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="E16" s="1">
         <v>0.24</v>
@@ -1953,14 +1945,14 @@
       <c r="A17">
         <v>1.2199999999999999E-3</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+      <c r="B17" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="E17" s="1">
         <v>0.24</v>
@@ -1986,7 +1978,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="E18" s="1">
         <v>0.24</v>
@@ -2012,7 +2004,7 @@
         <v>2.2699999999999999E-3</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="E19" s="1">
         <v>0.24</v>
@@ -2031,14 +2023,14 @@
       <c r="A20">
         <v>1.07E-3</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
+      <c r="B20" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.24</v>
       </c>
       <c r="E20" s="1">
         <v>0.24</v>
@@ -2057,14 +2049,14 @@
       <c r="A21">
         <v>1.2199999999999999E-3</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
+      <c r="B21" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.24</v>
       </c>
       <c r="E21" s="1">
         <v>0.24</v>
@@ -2240,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2395,8 +2387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,12 +2397,12 @@
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -2418,16 +2410,10 @@
       <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>5.5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2438,16 +2424,10 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>10.9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2458,16 +2438,10 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2">
-        <v>10.9</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0.3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2478,16 +2452,10 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1E-3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2498,16 +2466,10 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1.7</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2518,19 +2480,13 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2538,19 +2494,13 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="2">
-        <v>10</v>
-      </c>
-      <c r="H7" s="2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="2">
+        <v>500</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2558,19 +2508,13 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="2">
-        <v>100</v>
-      </c>
-      <c r="H8" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -2578,19 +2522,13 @@
       <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>10</v>
       </c>
-      <c r="H9" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" s="2">
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -2598,19 +2536,13 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="2">
-        <v>10</v>
-      </c>
-      <c r="H10" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
@@ -2618,19 +2550,13 @@
       <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="2">
-        <v>20</v>
-      </c>
-      <c r="H11" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>4.4710000000000001</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.4710000000000001</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -2638,19 +2564,14 @@
       <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="2">
-        <v>4.4710000000000001</v>
-      </c>
-      <c r="H12" s="2">
-        <v>4.4710000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.4079999999999999</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -2658,19 +2579,14 @@
       <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="2">
-        <v>1.4079999999999999</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1.4079999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3.4910000000000001</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.4910000000000001</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
@@ -2678,19 +2594,14 @@
       <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="2">
-        <v>3.4910000000000001</v>
-      </c>
-      <c r="H14" s="2">
-        <v>3.4910000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2.2120000000000002</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2.2120000000000002</v>
       </c>
       <c r="C15" t="s">
         <v>45</v>
@@ -2698,19 +2609,14 @@
       <c r="D15" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="2">
-        <v>2.2120000000000002</v>
-      </c>
-      <c r="H15" s="2">
-        <v>2.2120000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3.4609999999999999</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3.4609999999999999</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -2718,19 +2624,14 @@
       <c r="D16" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="2">
-        <v>3.4609999999999999</v>
-      </c>
-      <c r="H16" s="2">
-        <v>3.4609999999999999</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="A17" s="2">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.7629999999999999</v>
       </c>
       <c r="C17" t="s">
         <v>49</v>
@@ -2738,19 +2639,14 @@
       <c r="D17" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="2">
-        <v>2.7629999999999999</v>
-      </c>
-      <c r="H17" s="2">
-        <v>2.7629999999999999</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="A18" s="2">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.47199999999999998</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -2758,19 +2654,14 @@
       <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.47199999999999998</v>
-      </c>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="A19" s="2">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.2589999999999999</v>
       </c>
       <c r="C19" t="s">
         <v>53</v>
@@ -2778,19 +2669,14 @@
       <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="2">
-        <v>1.2589999999999999</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1.2589999999999999</v>
-      </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="A20" s="2">
+        <v>5.0979999999999999</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5.0979999999999999</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
@@ -2798,22 +2684,17 @@
       <c r="D20" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="2">
-        <v>5.0979999999999999</v>
-      </c>
-      <c r="H20" s="2">
-        <v>5.0979999999999999</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="A21" s="2">
+        <v>2.734</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.734</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -2821,18 +2702,13 @@
       <c r="D21" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="2">
-        <v>2.734</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2.734</v>
-      </c>
+      <c r="G21" s="2"/>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2843,12 +2719,6 @@
       <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
     </row>
@@ -2865,12 +2735,7 @@
       <c r="D23" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
+      <c r="G23" s="2"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2886,12 +2751,7 @@
       <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2906,12 +2766,7 @@
       <c r="D25" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2926,12 +2781,7 @@
       <c r="D26" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2946,12 +2796,7 @@
       <c r="D27" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -2966,16 +2811,11 @@
       <c r="D28" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -2986,12 +2826,6 @@
       <c r="D29" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -3006,12 +2840,7 @@
       <c r="D30" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1E-3</v>
-      </c>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -3026,12 +2855,7 @@
       <c r="D31" t="s">
         <v>79</v>
       </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -3046,12 +2870,7 @@
       <c r="D32" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -3071,7 +2890,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor update, running simulation with Sbo-Cancer
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7BF8F8E5-AAD6-45E4-B25B-142C4BAAF2A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE3AEA1C-EE71-4BC1-9B4A-7E1992935C46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="3" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -642,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B78F5ED-0798-4D77-8F9F-1DE91C850719}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q14:R15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,7 @@
     <col min="7" max="7" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -757,7 +757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -783,7 +783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -809,24 +809,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>8.9922067541464106</v>
+        <v>0.89922067541464101</v>
       </c>
       <c r="B7" s="1">
-        <v>8.9922067541464106</v>
+        <v>0.89922067541464101</v>
       </c>
       <c r="C7" s="1">
-        <v>8.9922067541464106</v>
+        <v>0.89922067541464101</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1.04895</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>1.04895</v>
+        <v>0.104895</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -835,7 +835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -861,7 +861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2.5</v>
       </c>
@@ -887,7 +887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -912,9 +912,8 @@
       <c r="H10" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.623</v>
       </c>
@@ -940,7 +939,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.2</v>
       </c>
@@ -951,7 +950,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D12">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E12">
         <v>0.20625000000000002</v>
@@ -966,7 +965,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.2</v>
       </c>
@@ -977,7 +976,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D13">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E13">
         <v>0.20625000000000002</v>
@@ -992,7 +991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.2</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D14">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E14">
         <v>0.20625000000000002</v>
@@ -1018,7 +1017,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.3</v>
       </c>
@@ -1029,7 +1028,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D15">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E15">
         <v>0.20625000000000002</v>
@@ -1044,7 +1043,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.56399999999999995</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D16">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E16">
         <v>0.20625000000000002</v>
@@ -1081,7 +1080,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D17">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E17">
         <v>0.20625000000000002</v>
@@ -1107,7 +1106,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="D18">
-        <v>2.0625</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="E18">
         <v>0.20625000000000002</v>
@@ -1133,7 +1132,7 @@
         <v>0.156</v>
       </c>
       <c r="D19">
-        <v>2.0625</v>
+        <v>0.156</v>
       </c>
       <c r="E19">
         <v>0.20625000000000002</v>
@@ -1159,7 +1158,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D20">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E20">
         <v>0.20625000000000002</v>
@@ -1185,7 +1184,7 @@
         <v>0.20625000000000002</v>
       </c>
       <c r="D21">
-        <v>2.0625</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="E21">
         <v>0.20625000000000002</v>
@@ -1357,23 +1356,23 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="A28" s="1">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1">
+        <v>10</v>
       </c>
       <c r="G28" t="s">
         <v>72</v>
@@ -1514,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A256C0EB-A98E-4A67-AA7F-D6B1D6307FBC}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K7" sqref="K7:P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1524,7 @@
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1551,7 +1550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1681,9 +1680,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.31084171495814739</v>
+        <v>3.1084171495814699E-2</v>
       </c>
       <c r="B7" s="1">
         <v>0.31084171495814739</v>
@@ -1706,8 +1705,14 @@
       <c r="H7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1E-3</v>
       </c>
@@ -1733,7 +1738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1758,8 +1763,9 @@
       <c r="H9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.157</v>
       </c>
@@ -1784,8 +1790,13 @@
       <c r="H10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1810,8 +1821,14 @@
       <c r="H11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -1836,8 +1853,13 @@
       <c r="H12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -1862,8 +1884,13 @@
       <c r="H13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -1888,8 +1915,13 @@
       <c r="H14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7.2000000000000005E-4</v>
       </c>
@@ -1914,8 +1946,13 @@
       <c r="H15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -1940,8 +1977,13 @@
       <c r="H16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -1966,8 +2008,13 @@
       <c r="H17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8.9999999999999998E-4</v>
       </c>
@@ -1992,8 +2039,10 @@
       <c r="H18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.2699999999999999E-3</v>
       </c>
@@ -2018,8 +2067,10 @@
       <c r="H19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.07E-3</v>
       </c>
@@ -2044,8 +2095,13 @@
       <c r="H20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.2199999999999999E-3</v>
       </c>
@@ -2070,8 +2126,13 @@
       <c r="H21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2096,8 +2157,11 @@
       <c r="H22" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N22" s="2"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2122,8 +2186,10 @@
       <c r="H23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2149,7 +2215,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2175,7 +2241,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2200,8 +2266,9 @@
       <c r="H26" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -2226,8 +2293,11 @@
       <c r="H27" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2253,7 +2323,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2279,7 +2349,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2305,7 +2375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2331,7 +2401,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -2388,7 +2458,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -2413,7 +2483,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2424,10 +2494,13 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
+      <c r="F2" s="2">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>10.9</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2438,10 +2511,13 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
+      <c r="F3" s="2">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2452,10 +2528,13 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="2">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2466,10 +2545,13 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
+      <c r="F5" s="2">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2500,7 +2582,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2511,7 +2593,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>50</v>
@@ -2542,7 +2624,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
@@ -2556,7 +2638,8 @@
         <v>4.4710000000000001</v>
       </c>
       <c r="B12" s="2">
-        <v>4.4710000000000001</v>
+        <f>A12*10</f>
+        <v>44.71</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -2571,7 +2654,8 @@
         <v>1.4079999999999999</v>
       </c>
       <c r="B13" s="2">
-        <v>1.4079999999999999</v>
+        <f t="shared" ref="B13:B21" si="0">A13*10</f>
+        <v>14.079999999999998</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -2586,7 +2670,8 @@
         <v>3.4910000000000001</v>
       </c>
       <c r="B14" s="2">
-        <v>3.4910000000000001</v>
+        <f t="shared" si="0"/>
+        <v>34.910000000000004</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
@@ -2601,7 +2686,8 @@
         <v>2.2120000000000002</v>
       </c>
       <c r="B15" s="2">
-        <v>2.2120000000000002</v>
+        <f t="shared" si="0"/>
+        <v>22.12</v>
       </c>
       <c r="C15" t="s">
         <v>45</v>
@@ -2616,7 +2702,8 @@
         <v>3.4609999999999999</v>
       </c>
       <c r="B16" s="2">
-        <v>3.4609999999999999</v>
+        <f t="shared" si="0"/>
+        <v>34.61</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -2631,7 +2718,8 @@
         <v>2.7629999999999999</v>
       </c>
       <c r="B17" s="2">
-        <v>2.7629999999999999</v>
+        <f t="shared" si="0"/>
+        <v>27.63</v>
       </c>
       <c r="C17" t="s">
         <v>49</v>
@@ -2646,7 +2734,8 @@
         <v>0.47199999999999998</v>
       </c>
       <c r="B18" s="2">
-        <v>0.47199999999999998</v>
+        <f t="shared" si="0"/>
+        <v>4.72</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -2661,7 +2750,8 @@
         <v>1.2589999999999999</v>
       </c>
       <c r="B19" s="2">
-        <v>1.2589999999999999</v>
+        <f t="shared" si="0"/>
+        <v>12.59</v>
       </c>
       <c r="C19" t="s">
         <v>53</v>
@@ -2676,7 +2766,8 @@
         <v>5.0979999999999999</v>
       </c>
       <c r="B20" s="2">
-        <v>5.0979999999999999</v>
+        <f t="shared" si="0"/>
+        <v>50.98</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
@@ -2694,7 +2785,8 @@
         <v>2.734</v>
       </c>
       <c r="B21" s="2">
-        <v>2.734</v>
+        <f t="shared" si="0"/>
+        <v>27.34</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -2889,8 +2981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C03891-79FA-45CB-ABD2-AD02C29D2916}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,7 +3008,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2946,7 +3038,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
minor changes to f() function file, updated kinetic parameters & intial conditions
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/Scripts/paramTables.xlsx
+++ b/iGEM simulation environment/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\iGEM simulation environment\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE3AEA1C-EE71-4BC1-9B4A-7E1992935C46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E37E46B-E54A-4BCB-B29F-CDE105CF09F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="3" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3645" windowHeight="345" activeTab="2" xr2:uid="{5BB18B0B-3499-4B48-8CA4-59B1E24E065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="84">
   <si>
     <t>sbo</t>
   </si>
@@ -277,12 +277,18 @@
   </si>
   <si>
     <t>x(12)</t>
+  </si>
+  <si>
+    <t>sbo-cancer long flows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,11 +329,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,7 +658,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,9 +830,9 @@
         <v>0.89922067541464101</v>
       </c>
       <c r="C7" s="1">
-        <v>0.89922067541464101</v>
-      </c>
-      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
         <v>0</v>
       </c>
       <c r="E7" s="1">
@@ -845,7 +858,7 @@
       <c r="C8">
         <v>1000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0</v>
       </c>
       <c r="E8">
@@ -2455,9 +2468,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F9859B-AB82-43CC-AE65-360143EE87F0}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2467,12 +2480,12 @@
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -2481,9 +2494,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>35</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2494,13 +2507,13 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2">
+      <c r="I2" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>0</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2511,13 +2524,13 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="2">
+      <c r="I3" s="2">
         <v>10.9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>0</v>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2.666666666666667</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2528,13 +2541,13 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2">
+      <c r="I4" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2545,11 +2558,11 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -2562,13 +2575,16 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>100</v>
+      <c r="B7" s="4">
+        <v>400</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2576,13 +2592,16 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>100</v>
-      </c>
-      <c r="B8" s="2">
         <v>1000</v>
+      </c>
+      <c r="B8" s="5">
+        <v>6000</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2590,13 +2609,16 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O8" s="2">
+        <v>190.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
-        <v>50</v>
+      <c r="B9" s="5">
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -2604,13 +2626,16 @@
       <c r="D9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O9" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
-        <v>200</v>
+      <c r="B10" s="4">
+        <v>600</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -2618,13 +2643,16 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O10" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>20</v>
       </c>
-      <c r="B11" s="2">
-        <v>100</v>
+      <c r="B11" s="4">
+        <v>464.01515151515156</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
@@ -2632,14 +2660,16 @@
       <c r="D11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O11" s="2">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>4.4710000000000001</v>
       </c>
-      <c r="B12" s="2">
-        <f>A12*10</f>
-        <v>44.71</v>
+      <c r="B12" s="4">
+        <v>14.727769753830806</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -2648,14 +2678,16 @@
         <v>42</v>
       </c>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O12" s="2">
+        <v>21.065000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1.4079999999999999</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" ref="B13:B21" si="0">A13*10</f>
-        <v>14.079999999999998</v>
+      <c r="B13" s="5">
+        <v>4.6376817793040894</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -2664,110 +2696,131 @@
         <v>44</v>
       </c>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O13" s="2">
+        <f t="shared" ref="O13:O22" si="0">A12*10</f>
+        <v>44.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3.4910000000000001</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
+        <v>11.499563351906998</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="O14" s="2">
+        <f t="shared" si="0"/>
+        <v>14.079999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2.2120000000000002</v>
+      </c>
+      <c r="B15" s="4">
+        <v>7.285514971851204</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="O15" s="2">
         <f t="shared" si="0"/>
         <v>34.910000000000004</v>
       </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2.2120000000000002</v>
-      </c>
-      <c r="B15" s="2">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3.4609999999999999</v>
+      </c>
+      <c r="B16" s="4">
+        <v>11.39965928698323</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="O16" s="2">
         <f t="shared" si="0"/>
         <v>22.12</v>
       </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>3.4609999999999999</v>
-      </c>
-      <c r="B16" s="2">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="B17" s="4">
+        <v>9.1008015542839527</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="O17" s="2">
         <f t="shared" si="0"/>
         <v>34.61</v>
       </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2.7629999999999999</v>
-      </c>
-      <c r="B17" s="2">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1.5540619819742105</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="O18" s="2">
         <f t="shared" si="0"/>
         <v>27.63</v>
       </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="B18" s="2">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="B19" s="4">
+        <v>4.1487143163816773</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="O19" s="2">
         <f t="shared" si="0"/>
         <v>4.72</v>
       </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1.2589999999999999</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>12.59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>5.0979999999999999</v>
       </c>
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>50.98</v>
+      <c r="B20" s="4">
+        <v>16.793017232500791</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
@@ -2779,14 +2832,17 @@
       <c r="K20" s="3"/>
       <c r="L20" s="2"/>
       <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O20" s="2">
+        <f t="shared" si="0"/>
+        <v>12.59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2.734</v>
       </c>
-      <c r="B21" s="2">
-        <f t="shared" si="0"/>
-        <v>27.34</v>
+      <c r="B21" s="5">
+        <v>9.0073815683599125</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -2797,8 +2853,12 @@
       <c r="G21" s="2"/>
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O21" s="2">
+        <f t="shared" si="0"/>
+        <v>50.98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2811,10 +2871,12 @@
       <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" s="2">
+        <f t="shared" si="0"/>
+        <v>27.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2828,9 +2890,8 @@
         <v>62</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2845,7 +2906,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2860,7 +2921,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2875,7 +2936,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2890,7 +2951,7 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2905,7 +2966,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2919,7 +2980,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2934,7 +2995,7 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2949,7 +3010,7 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -2974,6 +3035,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2981,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C03891-79FA-45CB-ABD2-AD02C29D2916}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>